<commit_message>
code done for exp data interleaved
</commit_message>
<xml_diff>
--- a/Interleaved-Christian/evap_N_circ_cross_couter_flow/tuning_exp_interleaved.xlsx
+++ b/Interleaved-Christian/evap_N_circ_cross_couter_flow/tuning_exp_interleaved.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="690" windowWidth="25725" windowHeight="14850"/>
+    <workbookView xWindow="0" yWindow="1035" windowWidth="25725" windowHeight="14850"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>baseline</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>phi_in</t>
+  </si>
+  <si>
+    <t>W fan_evap</t>
   </si>
 </sst>
 </file>
@@ -417,15 +420,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -444,8 +447,11 @@
       <c r="F1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -464,8 +470,11 @@
       <c r="F2">
         <v>27.23</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <v>0.77890000000000004</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -484,8 +493,11 @@
       <c r="F3">
         <v>27.22</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <v>0.76480000000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -504,8 +516,11 @@
       <c r="F4">
         <v>25.86</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <v>0.78010000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -524,8 +539,11 @@
       <c r="F5">
         <v>25.29</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <v>0.77859999999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -544,8 +562,11 @@
       <c r="F6">
         <v>27.51</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <v>0.76019999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -564,8 +585,11 @@
       <c r="F7">
         <v>29.73</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <v>0.76390000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -584,8 +608,11 @@
       <c r="F8">
         <v>29.95</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <v>0.76959999999999995</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -603,6 +630,9 @@
       </c>
       <c r="F9">
         <v>32.19</v>
+      </c>
+      <c r="G9">
+        <v>0.75470000000000004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>